<commit_message>
feat: fix database for juli
</commit_message>
<xml_diff>
--- a/DataConfig.xlsx
+++ b/DataConfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nisal\Documents\UiPath\balloonpay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AKyas\Desktop\balloonpay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60AE74D-1D6C-49B8-A9B3-E6C69CD6B43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72443F4B-AFFB-4C7C-A70D-A7831669D46A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5550" yWindow="2100" windowWidth="17385" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,13 @@
     <t>ChannelName</t>
   </si>
   <si>
-    <t>polkercrew</t>
-  </si>
-  <si>
-    <t>POLKER Crew</t>
-  </si>
-  <si>
-    <t>Hi, my name is Julio Qose and I'm the CEO of TipTok 😁 TipTok aims to become the Cryptocurrency for Social Media and the next $1 Billion Market Cap token. We have regular AMAs and the whole team is doxxed in the website. For more information on our fascinating roadmap and our upcoming Whitelist Presale visit our webiste at https://tiptok.finance/ and join our TG https://t.me/TipTok_Official. Join our movement and be part of something great.</t>
+    <t>Hi, my name is Julio Qose and I'm the CEO of TipTok 😁 TipTok aims to become the Cryptocurrency for Social Media and the next $1 Billion Market Cap token. We have regular AMAs and the whole team is doxxed in the website. For more information on our fascinating roadmap and our upcoming Whitelist Presale visit our website at https://tiptok.finance/ and join our TG https://t.me/TipTok_Official. Join our movement and be part of something great.</t>
+  </si>
+  <si>
+    <t>satoshistreetbets</t>
+  </si>
+  <si>
+    <t>SatoshiStreetBets</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,13 +413,13 @@
     </row>
     <row r="2" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="G2" s="3"/>
     </row>

</xml_diff>